<commit_message>
refactored to have all moving parts in teams.js
</commit_message>
<xml_diff>
--- a/data/ultiquiz_seed.xlsx
+++ b/data/ultiquiz_seed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielchen/Desktop/UltiQuiz/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AC60FD-A2A3-EE47-850C-9FE056C79E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17D26BD-34AF-204A-9C9C-0ECF7662910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,9 +280,6 @@
     <t>Texas,UT,TUFF</t>
   </si>
   <si>
-    <t>California,Cal-Berkeley,Cal Berkeley,Berkeley,Ursa Major</t>
-  </si>
-  <si>
     <t>Georgia,University of Georgia,UGA,Jojah</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>Slocore</t>
+  </si>
+  <si>
+    <t>California,Cal-Berkeley,Cal Berkeley,UC Berkeley,Berkeley,Ursa Major</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,7 +823,7 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
@@ -986,7 +986,7 @@
         <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1006,7 +1006,7 @@
         <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1026,7 +1026,7 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1046,7 +1046,7 @@
         <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -1066,7 +1066,7 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1086,7 +1086,7 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -1106,7 +1106,7 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
fixed id vs rank bug
</commit_message>
<xml_diff>
--- a/data/ultiquiz_seed.xlsx
+++ b/data/ultiquiz_seed.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -822,9 +822,49 @@
         <v>20</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>British Columbia</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Thunderbirds</v>
+      </c>
+      <c r="C22" t="str">
+        <v>British Columbia,UBC,TBirds,Thunderbirds</v>
+      </c>
+      <c r="D22" t="str">
+        <v>d1w</v>
+      </c>
+      <c r="E22" t="str">
+        <v>1</v>
+      </c>
+      <c r="F22" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Carleton College</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Syzygy</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Carleton,Syzygy</v>
+      </c>
+      <c r="D23" t="str">
+        <v>d1w</v>
+      </c>
+      <c r="E23" t="str">
+        <v>2</v>
+      </c>
+      <c r="F23" t="str">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>